<commit_message>
Created Sep folder and sheet in DIP
</commit_message>
<xml_diff>
--- a/static/excel/IDC.xlsx
+++ b/static/excel/IDC.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit\Documents\IDC\decisionmaker\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914CC001-E23C-4BCE-9EC1-037762754144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EFED9C-7624-4D76-BBCF-B8F798A1D77C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DIP" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -398,7 +398,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Sheets of All Subjects as well as First Preference
</commit_message>
<xml_diff>
--- a/static/excel/IDC.xlsx
+++ b/static/excel/IDC.xlsx
@@ -8,12 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit\Documents\IDC\decisionmaker\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EFED9C-7624-4D76-BBCF-B8F798A1D77C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB338EAC-2927-44F3-82A1-D3F9A472819F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIP" sheetId="1" r:id="rId1"/>
+    <sheet name="SA" sheetId="2" r:id="rId2"/>
+    <sheet name="SEO" sheetId="3" r:id="rId3"/>
+    <sheet name="UE" sheetId="4" r:id="rId4"/>
+    <sheet name="AIS" sheetId="5" r:id="rId5"/>
+    <sheet name="ACN" sheetId="6" r:id="rId6"/>
+    <sheet name="FP" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="15">
   <si>
     <t>1st Pref</t>
   </si>
@@ -397,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,4 +686,1720 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567ABD8E-6B29-4150-A386-3193F5560ECB}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <f>A2*J2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*K2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2*L2%</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>A2*M2%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="F2" s="1">
+        <f>A2*N2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <f>A2*O2%</f>
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(B2:G2)</f>
+        <v>17.993000000000002</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2">
+        <v>15.8</v>
+      </c>
+      <c r="K2">
+        <v>10.5</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>31.6</v>
+      </c>
+      <c r="N2">
+        <v>10.5</v>
+      </c>
+      <c r="O2">
+        <v>26.3</v>
+      </c>
+      <c r="P2">
+        <f>SUM(J2:O2)</f>
+        <v>94.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>A3*J3%</f>
+        <v>5.016</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3*K3%</f>
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <f>A3*L3%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="E3" s="1">
+        <f>A3*M3%</f>
+        <v>9.0060000000000002</v>
+      </c>
+      <c r="F3" s="1">
+        <f>A3*N3%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="G3" s="1">
+        <f>A3*O3%</f>
+        <v>12.008000000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H5" si="0">SUM(B3:G3)</f>
+        <v>37.049999999999997</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3">
+        <v>13.2</v>
+      </c>
+      <c r="K3">
+        <v>5.3</v>
+      </c>
+      <c r="L3">
+        <v>15.8</v>
+      </c>
+      <c r="M3">
+        <v>23.7</v>
+      </c>
+      <c r="N3">
+        <v>7.9</v>
+      </c>
+      <c r="O3">
+        <v>31.6</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="1">SUM(J3:O3)</f>
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4*J4%</f>
+        <v>5.9939999999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4*K4%</f>
+        <v>1.9980000000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <f>A4*L4%</f>
+        <v>11.988</v>
+      </c>
+      <c r="E4" s="1">
+        <f>A4*M4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <f>A4*N4%</f>
+        <v>7.0200000000000005</v>
+      </c>
+      <c r="G4" s="1">
+        <f>A4*O4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>53.028000000000006</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4">
+        <v>11.1</v>
+      </c>
+      <c r="K4">
+        <v>3.7</v>
+      </c>
+      <c r="L4">
+        <v>22.2</v>
+      </c>
+      <c r="M4">
+        <v>24.1</v>
+      </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+      <c r="O4">
+        <v>24.1</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>98.199999999999989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <f>A5*J5%</f>
+        <v>5.9850000000000003</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5*K5%</f>
+        <v>2.016</v>
+      </c>
+      <c r="D5" s="1">
+        <f>A5*L5%</f>
+        <v>18.018000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <f>A5*M5%</f>
+        <v>12.978000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5*N5%</f>
+        <v>8.0009999999999994</v>
+      </c>
+      <c r="G5" s="1">
+        <f>A5*O5%</f>
+        <v>14.994000000000002</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>61.991999999999997</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <v>9.5</v>
+      </c>
+      <c r="K5">
+        <v>3.2</v>
+      </c>
+      <c r="L5">
+        <v>28.6</v>
+      </c>
+      <c r="M5">
+        <v>20.6</v>
+      </c>
+      <c r="N5">
+        <v>12.7</v>
+      </c>
+      <c r="O5">
+        <v>23.8</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>98.399999999999991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A85909-6CCD-4362-9EE2-6E9E8CEA7FDD}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <f>A2*J2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*K2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2*L2%</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>A2*M2%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="F2" s="1">
+        <f>A2*N2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <f>A2*O2%</f>
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(B2:G2)</f>
+        <v>17.993000000000002</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2">
+        <v>15.8</v>
+      </c>
+      <c r="K2">
+        <v>10.5</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>31.6</v>
+      </c>
+      <c r="N2">
+        <v>10.5</v>
+      </c>
+      <c r="O2">
+        <v>26.3</v>
+      </c>
+      <c r="P2">
+        <f>SUM(J2:O2)</f>
+        <v>94.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>A3*J3%</f>
+        <v>5.016</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3*K3%</f>
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <f>A3*L3%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="E3" s="1">
+        <f>A3*M3%</f>
+        <v>9.0060000000000002</v>
+      </c>
+      <c r="F3" s="1">
+        <f>A3*N3%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="G3" s="1">
+        <f>A3*O3%</f>
+        <v>12.008000000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H5" si="0">SUM(B3:G3)</f>
+        <v>37.049999999999997</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3">
+        <v>13.2</v>
+      </c>
+      <c r="K3">
+        <v>5.3</v>
+      </c>
+      <c r="L3">
+        <v>15.8</v>
+      </c>
+      <c r="M3">
+        <v>23.7</v>
+      </c>
+      <c r="N3">
+        <v>7.9</v>
+      </c>
+      <c r="O3">
+        <v>31.6</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="1">SUM(J3:O3)</f>
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4*J4%</f>
+        <v>5.9939999999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4*K4%</f>
+        <v>1.9980000000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <f>A4*L4%</f>
+        <v>11.988</v>
+      </c>
+      <c r="E4" s="1">
+        <f>A4*M4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <f>A4*N4%</f>
+        <v>7.0200000000000005</v>
+      </c>
+      <c r="G4" s="1">
+        <f>A4*O4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>53.028000000000006</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4">
+        <v>11.1</v>
+      </c>
+      <c r="K4">
+        <v>3.7</v>
+      </c>
+      <c r="L4">
+        <v>22.2</v>
+      </c>
+      <c r="M4">
+        <v>24.1</v>
+      </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+      <c r="O4">
+        <v>24.1</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>98.199999999999989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <f>A5*J5%</f>
+        <v>5.9850000000000003</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5*K5%</f>
+        <v>2.016</v>
+      </c>
+      <c r="D5" s="1">
+        <f>A5*L5%</f>
+        <v>18.018000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <f>A5*M5%</f>
+        <v>12.978000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5*N5%</f>
+        <v>8.0009999999999994</v>
+      </c>
+      <c r="G5" s="1">
+        <f>A5*O5%</f>
+        <v>14.994000000000002</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>61.991999999999997</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <v>9.5</v>
+      </c>
+      <c r="K5">
+        <v>3.2</v>
+      </c>
+      <c r="L5">
+        <v>28.6</v>
+      </c>
+      <c r="M5">
+        <v>20.6</v>
+      </c>
+      <c r="N5">
+        <v>12.7</v>
+      </c>
+      <c r="O5">
+        <v>23.8</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>98.399999999999991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12545823-AC50-44A7-95B3-32618C72B466}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <f>A2*J2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*K2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2*L2%</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>A2*M2%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="F2" s="1">
+        <f>A2*N2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <f>A2*O2%</f>
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(B2:G2)</f>
+        <v>17.993000000000002</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2">
+        <v>15.8</v>
+      </c>
+      <c r="K2">
+        <v>10.5</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>31.6</v>
+      </c>
+      <c r="N2">
+        <v>10.5</v>
+      </c>
+      <c r="O2">
+        <v>26.3</v>
+      </c>
+      <c r="P2">
+        <f>SUM(J2:O2)</f>
+        <v>94.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>A3*J3%</f>
+        <v>5.016</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3*K3%</f>
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <f>A3*L3%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="E3" s="1">
+        <f>A3*M3%</f>
+        <v>9.0060000000000002</v>
+      </c>
+      <c r="F3" s="1">
+        <f>A3*N3%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="G3" s="1">
+        <f>A3*O3%</f>
+        <v>12.008000000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H5" si="0">SUM(B3:G3)</f>
+        <v>37.049999999999997</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3">
+        <v>13.2</v>
+      </c>
+      <c r="K3">
+        <v>5.3</v>
+      </c>
+      <c r="L3">
+        <v>15.8</v>
+      </c>
+      <c r="M3">
+        <v>23.7</v>
+      </c>
+      <c r="N3">
+        <v>7.9</v>
+      </c>
+      <c r="O3">
+        <v>31.6</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="1">SUM(J3:O3)</f>
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4*J4%</f>
+        <v>5.9939999999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4*K4%</f>
+        <v>1.9980000000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <f>A4*L4%</f>
+        <v>11.988</v>
+      </c>
+      <c r="E4" s="1">
+        <f>A4*M4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <f>A4*N4%</f>
+        <v>7.0200000000000005</v>
+      </c>
+      <c r="G4" s="1">
+        <f>A4*O4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>53.028000000000006</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4">
+        <v>11.1</v>
+      </c>
+      <c r="K4">
+        <v>3.7</v>
+      </c>
+      <c r="L4">
+        <v>22.2</v>
+      </c>
+      <c r="M4">
+        <v>24.1</v>
+      </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+      <c r="O4">
+        <v>24.1</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>98.199999999999989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <f>A5*J5%</f>
+        <v>5.9850000000000003</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5*K5%</f>
+        <v>2.016</v>
+      </c>
+      <c r="D5" s="1">
+        <f>A5*L5%</f>
+        <v>18.018000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <f>A5*M5%</f>
+        <v>12.978000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5*N5%</f>
+        <v>8.0009999999999994</v>
+      </c>
+      <c r="G5" s="1">
+        <f>A5*O5%</f>
+        <v>14.994000000000002</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>61.991999999999997</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <v>9.5</v>
+      </c>
+      <c r="K5">
+        <v>3.2</v>
+      </c>
+      <c r="L5">
+        <v>28.6</v>
+      </c>
+      <c r="M5">
+        <v>20.6</v>
+      </c>
+      <c r="N5">
+        <v>12.7</v>
+      </c>
+      <c r="O5">
+        <v>23.8</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>98.399999999999991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8FEF25-1CAB-4ADA-8340-9581040D1F17}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <f>A2*J2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*K2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2*L2%</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>A2*M2%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="F2" s="1">
+        <f>A2*N2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <f>A2*O2%</f>
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(B2:G2)</f>
+        <v>17.993000000000002</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2">
+        <v>15.8</v>
+      </c>
+      <c r="K2">
+        <v>10.5</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>31.6</v>
+      </c>
+      <c r="N2">
+        <v>10.5</v>
+      </c>
+      <c r="O2">
+        <v>26.3</v>
+      </c>
+      <c r="P2">
+        <f>SUM(J2:O2)</f>
+        <v>94.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>A3*J3%</f>
+        <v>5.016</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3*K3%</f>
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <f>A3*L3%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="E3" s="1">
+        <f>A3*M3%</f>
+        <v>9.0060000000000002</v>
+      </c>
+      <c r="F3" s="1">
+        <f>A3*N3%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="G3" s="1">
+        <f>A3*O3%</f>
+        <v>12.008000000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H5" si="0">SUM(B3:G3)</f>
+        <v>37.049999999999997</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3">
+        <v>13.2</v>
+      </c>
+      <c r="K3">
+        <v>5.3</v>
+      </c>
+      <c r="L3">
+        <v>15.8</v>
+      </c>
+      <c r="M3">
+        <v>23.7</v>
+      </c>
+      <c r="N3">
+        <v>7.9</v>
+      </c>
+      <c r="O3">
+        <v>31.6</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="1">SUM(J3:O3)</f>
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4*J4%</f>
+        <v>5.9939999999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4*K4%</f>
+        <v>1.9980000000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <f>A4*L4%</f>
+        <v>11.988</v>
+      </c>
+      <c r="E4" s="1">
+        <f>A4*M4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <f>A4*N4%</f>
+        <v>7.0200000000000005</v>
+      </c>
+      <c r="G4" s="1">
+        <f>A4*O4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>53.028000000000006</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4">
+        <v>11.1</v>
+      </c>
+      <c r="K4">
+        <v>3.7</v>
+      </c>
+      <c r="L4">
+        <v>22.2</v>
+      </c>
+      <c r="M4">
+        <v>24.1</v>
+      </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+      <c r="O4">
+        <v>24.1</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>98.199999999999989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <f>A5*J5%</f>
+        <v>5.9850000000000003</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5*K5%</f>
+        <v>2.016</v>
+      </c>
+      <c r="D5" s="1">
+        <f>A5*L5%</f>
+        <v>18.018000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <f>A5*M5%</f>
+        <v>12.978000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5*N5%</f>
+        <v>8.0009999999999994</v>
+      </c>
+      <c r="G5" s="1">
+        <f>A5*O5%</f>
+        <v>14.994000000000002</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>61.991999999999997</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <v>9.5</v>
+      </c>
+      <c r="K5">
+        <v>3.2</v>
+      </c>
+      <c r="L5">
+        <v>28.6</v>
+      </c>
+      <c r="M5">
+        <v>20.6</v>
+      </c>
+      <c r="N5">
+        <v>12.7</v>
+      </c>
+      <c r="O5">
+        <v>23.8</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>98.399999999999991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B453A48-6FCC-4751-8C13-6B4691430F6E}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <f>A2*J2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*K2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2*L2%</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>A2*M2%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="F2" s="1">
+        <f>A2*N2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <f>A2*O2%</f>
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(B2:G2)</f>
+        <v>17.993000000000002</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2">
+        <v>15.8</v>
+      </c>
+      <c r="K2">
+        <v>10.5</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>31.6</v>
+      </c>
+      <c r="N2">
+        <v>10.5</v>
+      </c>
+      <c r="O2">
+        <v>26.3</v>
+      </c>
+      <c r="P2">
+        <f>SUM(J2:O2)</f>
+        <v>94.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>A3*J3%</f>
+        <v>5.016</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3*K3%</f>
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <f>A3*L3%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="E3" s="1">
+        <f>A3*M3%</f>
+        <v>9.0060000000000002</v>
+      </c>
+      <c r="F3" s="1">
+        <f>A3*N3%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="G3" s="1">
+        <f>A3*O3%</f>
+        <v>12.008000000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H5" si="0">SUM(B3:G3)</f>
+        <v>37.049999999999997</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3">
+        <v>13.2</v>
+      </c>
+      <c r="K3">
+        <v>5.3</v>
+      </c>
+      <c r="L3">
+        <v>15.8</v>
+      </c>
+      <c r="M3">
+        <v>23.7</v>
+      </c>
+      <c r="N3">
+        <v>7.9</v>
+      </c>
+      <c r="O3">
+        <v>31.6</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="1">SUM(J3:O3)</f>
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4*J4%</f>
+        <v>5.9939999999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4*K4%</f>
+        <v>1.9980000000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <f>A4*L4%</f>
+        <v>11.988</v>
+      </c>
+      <c r="E4" s="1">
+        <f>A4*M4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <f>A4*N4%</f>
+        <v>7.0200000000000005</v>
+      </c>
+      <c r="G4" s="1">
+        <f>A4*O4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>53.028000000000006</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4">
+        <v>11.1</v>
+      </c>
+      <c r="K4">
+        <v>3.7</v>
+      </c>
+      <c r="L4">
+        <v>22.2</v>
+      </c>
+      <c r="M4">
+        <v>24.1</v>
+      </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+      <c r="O4">
+        <v>24.1</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>98.199999999999989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <f>A5*J5%</f>
+        <v>5.9850000000000003</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5*K5%</f>
+        <v>2.016</v>
+      </c>
+      <c r="D5" s="1">
+        <f>A5*L5%</f>
+        <v>18.018000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <f>A5*M5%</f>
+        <v>12.978000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5*N5%</f>
+        <v>8.0009999999999994</v>
+      </c>
+      <c r="G5" s="1">
+        <f>A5*O5%</f>
+        <v>14.994000000000002</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>61.991999999999997</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <v>9.5</v>
+      </c>
+      <c r="K5">
+        <v>3.2</v>
+      </c>
+      <c r="L5">
+        <v>28.6</v>
+      </c>
+      <c r="M5">
+        <v>20.6</v>
+      </c>
+      <c r="N5">
+        <v>12.7</v>
+      </c>
+      <c r="O5">
+        <v>23.8</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>98.399999999999991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312D2B4B-65DA-4A16-B682-41207C4E444E}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <f>A2*J2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*K2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2*L2%</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>A2*M2%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="F2" s="1">
+        <f>A2*N2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <f>A2*O2%</f>
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(B2:G2)</f>
+        <v>17.993000000000002</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2">
+        <v>15.8</v>
+      </c>
+      <c r="K2">
+        <v>10.5</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>31.6</v>
+      </c>
+      <c r="N2">
+        <v>10.5</v>
+      </c>
+      <c r="O2">
+        <v>26.3</v>
+      </c>
+      <c r="P2">
+        <f>SUM(J2:O2)</f>
+        <v>94.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>A3*J3%</f>
+        <v>5.016</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3*K3%</f>
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <f>A3*L3%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="E3" s="1">
+        <f>A3*M3%</f>
+        <v>9.0060000000000002</v>
+      </c>
+      <c r="F3" s="1">
+        <f>A3*N3%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="G3" s="1">
+        <f>A3*O3%</f>
+        <v>12.008000000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H5" si="0">SUM(B3:G3)</f>
+        <v>37.049999999999997</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3">
+        <v>13.2</v>
+      </c>
+      <c r="K3">
+        <v>5.3</v>
+      </c>
+      <c r="L3">
+        <v>15.8</v>
+      </c>
+      <c r="M3">
+        <v>23.7</v>
+      </c>
+      <c r="N3">
+        <v>7.9</v>
+      </c>
+      <c r="O3">
+        <v>31.6</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="1">SUM(J3:O3)</f>
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4*J4%</f>
+        <v>5.9939999999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4*K4%</f>
+        <v>1.9980000000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <f>A4*L4%</f>
+        <v>11.988</v>
+      </c>
+      <c r="E4" s="1">
+        <f>A4*M4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <f>A4*N4%</f>
+        <v>7.0200000000000005</v>
+      </c>
+      <c r="G4" s="1">
+        <f>A4*O4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>53.028000000000006</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4">
+        <v>11.1</v>
+      </c>
+      <c r="K4">
+        <v>3.7</v>
+      </c>
+      <c r="L4">
+        <v>22.2</v>
+      </c>
+      <c r="M4">
+        <v>24.1</v>
+      </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+      <c r="O4">
+        <v>24.1</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>98.199999999999989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <f>A5*J5%</f>
+        <v>5.9850000000000003</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5*K5%</f>
+        <v>2.016</v>
+      </c>
+      <c r="D5" s="1">
+        <f>A5*L5%</f>
+        <v>18.018000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <f>A5*M5%</f>
+        <v>12.978000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5*N5%</f>
+        <v>8.0009999999999994</v>
+      </c>
+      <c r="G5" s="1">
+        <f>A5*O5%</f>
+        <v>14.994000000000002</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>61.991999999999997</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <v>9.5</v>
+      </c>
+      <c r="K5">
+        <v>3.2</v>
+      </c>
+      <c r="L5">
+        <v>28.6</v>
+      </c>
+      <c r="M5">
+        <v>20.6</v>
+      </c>
+      <c r="N5">
+        <v>12.7</v>
+      </c>
+      <c r="O5">
+        <v>23.8</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>98.399999999999991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Data for second preference
</commit_message>
<xml_diff>
--- a/static/excel/IDC.xlsx
+++ b/static/excel/IDC.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit\Documents\IDC\decisionmaker\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D4A41F-2F19-4930-B470-C45B5E422042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED34C395-CDD9-43CF-AD36-4645BFADB849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIP" sheetId="1" r:id="rId1"/>
     <sheet name="FP" sheetId="7" r:id="rId2"/>
+    <sheet name="SP" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>1st Pref</t>
   </si>
@@ -706,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312D2B4B-65DA-4A16-B682-41207C4E444E}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,4 +990,287 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE7E77F-95DD-4B10-83E4-041B3BBF5D3C}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <f>A2*J2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*K2%</f>
+        <v>7.9990000000000006</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2*L2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="E2" s="1">
+        <f>A2*M2%</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <f>A2*N2%</f>
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <f>A2*O2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(B2:G2)</f>
+        <v>18.980999999999998</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2">
+        <v>10.5</v>
+      </c>
+      <c r="K2">
+        <v>42.1</v>
+      </c>
+      <c r="L2">
+        <v>10.5</v>
+      </c>
+      <c r="N2">
+        <v>26.3</v>
+      </c>
+      <c r="O2">
+        <v>10.5</v>
+      </c>
+      <c r="P2">
+        <f>SUM(J2:O2)</f>
+        <v>99.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>A3*J3%</f>
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3*K3%</f>
+        <v>9.9939999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <f>A3*L3%</f>
+        <v>3.9899999999999998</v>
+      </c>
+      <c r="E3" s="1">
+        <f>A3*M3%</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <f>A3*N3%</f>
+        <v>19</v>
+      </c>
+      <c r="G3" s="1">
+        <f>A3*O3%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H5" si="0">SUM(B3:G3)</f>
+        <v>38</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3">
+        <v>5.3</v>
+      </c>
+      <c r="K3">
+        <v>26.3</v>
+      </c>
+      <c r="L3">
+        <v>10.5</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>50</v>
+      </c>
+      <c r="O3">
+        <v>7.9</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="1">SUM(J3:O3)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4*J4%</f>
+        <v>1.9980000000000002</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4*K4%</f>
+        <v>9.99</v>
+      </c>
+      <c r="D4" s="1">
+        <f>A4*L4%</f>
+        <v>5.9939999999999998</v>
+      </c>
+      <c r="E4" s="1">
+        <f>A4*M4%</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <f>A4*N4%</f>
+        <v>30.024000000000001</v>
+      </c>
+      <c r="G4" s="1">
+        <f>A4*O4%</f>
+        <v>5.9939999999999998</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4">
+        <v>3.7</v>
+      </c>
+      <c r="K4">
+        <v>18.5</v>
+      </c>
+      <c r="L4">
+        <v>11.1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>55.6</v>
+      </c>
+      <c r="O4">
+        <v>11.1</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <f>A5*J5%</f>
+        <v>2.016</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5*K5%</f>
+        <v>10.016999999999999</v>
+      </c>
+      <c r="D5" s="1">
+        <f>A5*L5%</f>
+        <v>6.9930000000000003</v>
+      </c>
+      <c r="E5" s="1">
+        <f>A5*M5%</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5*N5%</f>
+        <v>37.988999999999997</v>
+      </c>
+      <c r="G5" s="1">
+        <f>A5*O5%</f>
+        <v>5.9850000000000003</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <v>3.2</v>
+      </c>
+      <c r="K5">
+        <v>15.9</v>
+      </c>
+      <c r="L5">
+        <v>11.1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>60.3</v>
+      </c>
+      <c r="O5">
+        <v>9.5</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Data for third preference
</commit_message>
<xml_diff>
--- a/static/excel/IDC.xlsx
+++ b/static/excel/IDC.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit\Documents\IDC\decisionmaker\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED34C395-CDD9-43CF-AD36-4645BFADB849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD66A23-A780-4121-8D1D-4E1E3C5F0734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIP" sheetId="1" r:id="rId1"/>
     <sheet name="FP" sheetId="7" r:id="rId2"/>
     <sheet name="SP" sheetId="8" r:id="rId3"/>
+    <sheet name="TP" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
   <si>
     <t>1st Pref</t>
   </si>
@@ -996,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE7E77F-95DD-4B10-83E4-041B3BBF5D3C}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1068,7 @@
       </c>
       <c r="E2" s="1">
         <f>A2*M2%</f>
-        <v>0</v>
+        <v>1.9E-2</v>
       </c>
       <c r="F2" s="1">
         <f>A2*N2%</f>
@@ -1079,7 +1080,7 @@
       </c>
       <c r="H2" s="1">
         <f>SUM(B2:G2)</f>
-        <v>18.980999999999998</v>
+        <v>19</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2">
@@ -1091,6 +1092,9 @@
       <c r="L2">
         <v>10.5</v>
       </c>
+      <c r="M2">
+        <v>0.1</v>
+      </c>
       <c r="N2">
         <v>26.3</v>
       </c>
@@ -1099,7 +1103,7 @@
       </c>
       <c r="P2">
         <f>SUM(J2:O2)</f>
-        <v>99.9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1268,6 +1272,292 @@
       <c r="P5">
         <f t="shared" si="1"/>
         <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59225AD-4E49-4CB8-BC4D-705EABA206D1}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <f>A2*J2%</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*K2%</f>
+        <v>4.0090000000000003</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2*L2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="E2" s="1">
+        <f>A2*M2%</f>
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <f>A2*N2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="G2" s="1">
+        <f>A2*O2%</f>
+        <v>4.0090000000000003</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(B2:G2)</f>
+        <v>19.019000000000002</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>21.1</v>
+      </c>
+      <c r="L2">
+        <v>15.8</v>
+      </c>
+      <c r="M2">
+        <v>26.3</v>
+      </c>
+      <c r="N2">
+        <v>15.8</v>
+      </c>
+      <c r="O2">
+        <v>21.1</v>
+      </c>
+      <c r="P2">
+        <f>SUM(J2:O2)</f>
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>A3*J3%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3*K3%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="D3" s="1">
+        <f>A3*L3%</f>
+        <v>3.9899999999999998</v>
+      </c>
+      <c r="E3" s="1">
+        <f>A3*M3%</f>
+        <v>9.0060000000000002</v>
+      </c>
+      <c r="F3" s="1">
+        <f>A3*N3%</f>
+        <v>5.016</v>
+      </c>
+      <c r="G3" s="1">
+        <f>A3*O3%</f>
+        <v>8.0180000000000007</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H5" si="0">SUM(B3:G3)</f>
+        <v>38.038000000000004</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3">
+        <v>15.8</v>
+      </c>
+      <c r="K3">
+        <v>15.8</v>
+      </c>
+      <c r="L3">
+        <v>10.5</v>
+      </c>
+      <c r="M3">
+        <v>23.7</v>
+      </c>
+      <c r="N3">
+        <v>13.2</v>
+      </c>
+      <c r="O3">
+        <v>21.1</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="1">SUM(J3:O3)</f>
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4*J4%</f>
+        <v>11.988</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4*K4%</f>
+        <v>7.9920000000000009</v>
+      </c>
+      <c r="D4" s="1">
+        <f>A4*L4%</f>
+        <v>7.9920000000000009</v>
+      </c>
+      <c r="E4" s="1">
+        <f>A4*M4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <f>A4*N4%</f>
+        <v>5.0220000000000011</v>
+      </c>
+      <c r="G4" s="1">
+        <f>A4*O4%</f>
+        <v>7.9920000000000009</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4">
+        <v>22.2</v>
+      </c>
+      <c r="K4">
+        <v>14.8</v>
+      </c>
+      <c r="L4">
+        <v>14.8</v>
+      </c>
+      <c r="M4">
+        <v>24.1</v>
+      </c>
+      <c r="N4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="O4">
+        <v>14.8</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <f>A5*J5%</f>
+        <v>18.018000000000001</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5*K5%</f>
+        <v>9.0090000000000003</v>
+      </c>
+      <c r="D5" s="1">
+        <f>A5*L5%</f>
+        <v>8.0009999999999994</v>
+      </c>
+      <c r="E5" s="1">
+        <f>A5*M5%</f>
+        <v>14.994000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5*N5%</f>
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="G5" s="1">
+        <f>A5*O5%</f>
+        <v>8.0009999999999994</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>62.999999999999993</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <v>28.6</v>
+      </c>
+      <c r="K5">
+        <v>14.3</v>
+      </c>
+      <c r="L5">
+        <v>12.7</v>
+      </c>
+      <c r="M5">
+        <v>23.8</v>
+      </c>
+      <c r="N5">
+        <v>7.9</v>
+      </c>
+      <c r="O5">
+        <v>12.7</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>100.00000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Data for fourth preference
</commit_message>
<xml_diff>
--- a/static/excel/IDC.xlsx
+++ b/static/excel/IDC.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit\Documents\IDC\decisionmaker\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD66A23-A780-4121-8D1D-4E1E3C5F0734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF9E6E6-C555-4F89-8838-25407DA1AF63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIP" sheetId="1" r:id="rId1"/>
     <sheet name="FP" sheetId="7" r:id="rId2"/>
     <sheet name="SP" sheetId="8" r:id="rId3"/>
     <sheet name="TP" sheetId="9" r:id="rId4"/>
+    <sheet name="FoP" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="21">
   <si>
     <t>1st Pref</t>
   </si>
@@ -1283,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59225AD-4E49-4CB8-BC4D-705EABA206D1}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,4 +1564,290 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6ECE78-ECAB-4BF0-A9D2-F1C8D49456BF}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <f>A2*J2%</f>
+        <v>6.0040000000000004</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*K2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2*L2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="E2" s="1">
+        <f>A2*M2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <f>A2*N2%</f>
+        <v>4.0090000000000003</v>
+      </c>
+      <c r="G2" s="1">
+        <f>A2*O2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(B2:G2)</f>
+        <v>19</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2">
+        <v>31.6</v>
+      </c>
+      <c r="K2">
+        <v>15.8</v>
+      </c>
+      <c r="L2">
+        <v>10.5</v>
+      </c>
+      <c r="M2">
+        <v>10.5</v>
+      </c>
+      <c r="N2">
+        <v>21.1</v>
+      </c>
+      <c r="O2">
+        <v>10.5</v>
+      </c>
+      <c r="P2">
+        <f>SUM(J2:O2)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>A3*J3%</f>
+        <v>9.0060000000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3*K3%</f>
+        <v>10.981999999999999</v>
+      </c>
+      <c r="D3" s="1">
+        <f>A3*L3%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="E3" s="1">
+        <f>A3*M3%</f>
+        <v>8.0180000000000007</v>
+      </c>
+      <c r="F3" s="1">
+        <f>A3*N3%</f>
+        <v>3.9899999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <f>A3*O3%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H5" si="0">SUM(B3:G3)</f>
+        <v>38</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3">
+        <v>23.7</v>
+      </c>
+      <c r="K3">
+        <v>28.9</v>
+      </c>
+      <c r="L3">
+        <v>7.9</v>
+      </c>
+      <c r="M3">
+        <v>21.1</v>
+      </c>
+      <c r="N3">
+        <v>10.5</v>
+      </c>
+      <c r="O3">
+        <v>7.9</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="1">SUM(J3:O3)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4*J4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4*K4%</f>
+        <v>17.010000000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <f>A4*L4%</f>
+        <v>2.97</v>
+      </c>
+      <c r="E4" s="1">
+        <f>A4*M4%</f>
+        <v>11.016</v>
+      </c>
+      <c r="F4" s="1">
+        <f>A4*N4%</f>
+        <v>7.0200000000000005</v>
+      </c>
+      <c r="G4" s="1">
+        <f>A4*O4%</f>
+        <v>2.97</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4">
+        <v>24.1</v>
+      </c>
+      <c r="K4">
+        <v>31.5</v>
+      </c>
+      <c r="L4">
+        <v>5.5</v>
+      </c>
+      <c r="M4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+      <c r="O4">
+        <v>5.5</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <f>A5*J5%</f>
+        <v>12.978000000000002</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5*K5%</f>
+        <v>19.026</v>
+      </c>
+      <c r="D5" s="1">
+        <f>A5*L5%</f>
+        <v>3.024</v>
+      </c>
+      <c r="E5" s="1">
+        <f>A5*M5%</f>
+        <v>17.010000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5*N5%</f>
+        <v>6.9930000000000003</v>
+      </c>
+      <c r="G5" s="1">
+        <f>A5*O5%</f>
+        <v>3.9689999999999999</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>63.000000000000014</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <v>20.6</v>
+      </c>
+      <c r="K5">
+        <v>30.2</v>
+      </c>
+      <c r="L5">
+        <v>4.8</v>
+      </c>
+      <c r="M5">
+        <v>27</v>
+      </c>
+      <c r="N5">
+        <v>11.1</v>
+      </c>
+      <c r="O5">
+        <v>6.3</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>99.999999999999986</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Data for fifth preference
</commit_message>
<xml_diff>
--- a/static/excel/IDC.xlsx
+++ b/static/excel/IDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit\Documents\IDC\decisionmaker\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF9E6E6-C555-4F89-8838-25407DA1AF63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA5AD0B-6FA6-4F6D-97C5-9287AB22494A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIP" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="SP" sheetId="8" r:id="rId3"/>
     <sheet name="TP" sheetId="9" r:id="rId4"/>
     <sheet name="FoP" sheetId="10" r:id="rId5"/>
+    <sheet name="FiP" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
   <si>
     <t>1st Pref</t>
   </si>
@@ -1570,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6ECE78-ECAB-4BF0-A9D2-F1C8D49456BF}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,4 +1851,290 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF3A003-6591-43A0-AC06-C46B170D979B}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <f>A2*J2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*K2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2*L2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="E2" s="1">
+        <f>A2*M2%</f>
+        <v>6.992</v>
+      </c>
+      <c r="F2" s="1">
+        <f>A2*N2%</f>
+        <v>1.0069999999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <f>A2*O2%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(B2:G2)</f>
+        <v>19</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2">
+        <v>10.5</v>
+      </c>
+      <c r="K2">
+        <v>15.8</v>
+      </c>
+      <c r="L2">
+        <v>15.8</v>
+      </c>
+      <c r="M2">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="N2">
+        <v>5.3</v>
+      </c>
+      <c r="O2">
+        <v>15.8</v>
+      </c>
+      <c r="P2">
+        <f>SUM(J2:O2)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>A3*J3%</f>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3*K3%</f>
+        <v>9.9939999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <f>A3*L3%</f>
+        <v>3.9899999999999998</v>
+      </c>
+      <c r="E3" s="1">
+        <f>A3*M3%</f>
+        <v>12.996</v>
+      </c>
+      <c r="F3" s="1">
+        <f>A3*N3%</f>
+        <v>1.026</v>
+      </c>
+      <c r="G3" s="1">
+        <f>A3*O3%</f>
+        <v>6.992</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H5" si="0">SUM(B3:G3)</f>
+        <v>38</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3">
+        <v>7.9</v>
+      </c>
+      <c r="K3">
+        <v>26.3</v>
+      </c>
+      <c r="L3">
+        <v>10.5</v>
+      </c>
+      <c r="M3">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="N3">
+        <v>2.7</v>
+      </c>
+      <c r="O3">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="1">SUM(J3:O3)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4*J4%</f>
+        <v>7.0200000000000005</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4*K4%</f>
+        <v>15.012</v>
+      </c>
+      <c r="D4" s="1">
+        <f>A4*L4%</f>
+        <v>3.7260000000000004</v>
+      </c>
+      <c r="E4" s="1">
+        <f>A4*M4%</f>
+        <v>17.010000000000002</v>
+      </c>
+      <c r="F4" s="1">
+        <f>A4*N4%</f>
+        <v>1.242</v>
+      </c>
+      <c r="G4" s="1">
+        <f>A4*O4%</f>
+        <v>9.99</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4">
+        <v>13</v>
+      </c>
+      <c r="K4">
+        <v>27.8</v>
+      </c>
+      <c r="L4">
+        <v>6.9</v>
+      </c>
+      <c r="M4">
+        <v>31.5</v>
+      </c>
+      <c r="N4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O4">
+        <v>18.5</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>99.999999999999986</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <f>A5*J5%</f>
+        <v>8.0009999999999994</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5*K5%</f>
+        <v>16.001999999999999</v>
+      </c>
+      <c r="D5" s="1">
+        <f>A5*L5%</f>
+        <v>3.7170000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <f>A5*M5%</f>
+        <v>17.010000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5*N5%</f>
+        <v>1.26</v>
+      </c>
+      <c r="G5" s="1">
+        <f>A5*O5%</f>
+        <v>17.010000000000002</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <v>12.7</v>
+      </c>
+      <c r="K5">
+        <v>25.4</v>
+      </c>
+      <c r="L5">
+        <v>5.9</v>
+      </c>
+      <c r="M5">
+        <v>27</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>27</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Data for sixth preference
</commit_message>
<xml_diff>
--- a/static/excel/IDC.xlsx
+++ b/static/excel/IDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit\Documents\IDC\decisionmaker\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA5AD0B-6FA6-4F6D-97C5-9287AB22494A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6A1566-0BF1-4E15-BD62-14E6ABD96F5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIP" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="TP" sheetId="9" r:id="rId4"/>
     <sheet name="FoP" sheetId="10" r:id="rId5"/>
     <sheet name="FiP" sheetId="11" r:id="rId6"/>
+    <sheet name="SiP" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="24">
   <si>
     <t>1st Pref</t>
   </si>
@@ -99,6 +100,15 @@
   </si>
   <si>
     <t>ACN</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -1857,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF3A003-6591-43A0-AC06-C46B170D979B}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,4 +2147,296 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A16B396-E65E-4B47-B1DE-118E1660A500}">
+  <dimension ref="A1:P9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <f>A2*J2%</f>
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <f>A2*K2%</f>
+        <v>1.9949999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2*L2%</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>A2*M2%</f>
+        <v>4.0090000000000003</v>
+      </c>
+      <c r="F2" s="1">
+        <f>A2*N2%</f>
+        <v>1.0069999999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <f>A2*O2%</f>
+        <v>6.992</v>
+      </c>
+      <c r="H2" s="1">
+        <f>SUM(B2:G2)</f>
+        <v>19</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2">
+        <v>26.3</v>
+      </c>
+      <c r="K2">
+        <v>10.5</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>21.1</v>
+      </c>
+      <c r="N2">
+        <v>5.3</v>
+      </c>
+      <c r="O2">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="P2">
+        <f>SUM(J2:O2)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <f>A3*J3%</f>
+        <v>12.008000000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3*K3%</f>
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <f>A3*L3%</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <f>A3*M3%</f>
+        <v>6.992</v>
+      </c>
+      <c r="F3" s="1">
+        <f>A3*N3%</f>
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <f>A3*O3%</f>
+        <v>15.010000000000002</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H5" si="0">SUM(B3:G3)</f>
+        <v>38.037999999999997</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3">
+        <v>31.6</v>
+      </c>
+      <c r="K3">
+        <v>5.3</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="N3">
+        <v>5.3</v>
+      </c>
+      <c r="O3">
+        <v>39.5</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="1">SUM(J3:O3)</f>
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4*J4%</f>
+        <v>13.014000000000001</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4*K4%</f>
+        <v>1.9980000000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <f>A4*L4%</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f>A4*M4%</f>
+        <v>11.988</v>
+      </c>
+      <c r="F4" s="1">
+        <f>A4*N4%</f>
+        <v>1.9980000000000002</v>
+      </c>
+      <c r="G4" s="1">
+        <f>A4*O4%</f>
+        <v>25.001999999999999</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4">
+        <v>24.1</v>
+      </c>
+      <c r="K4">
+        <v>3.7</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>22.2</v>
+      </c>
+      <c r="N4">
+        <v>3.7</v>
+      </c>
+      <c r="O4">
+        <v>46.3</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1">
+        <f>A5*J5%</f>
+        <v>14.994000000000002</v>
+      </c>
+      <c r="C5" s="1">
+        <f>A5*K5%</f>
+        <v>6.9930000000000003</v>
+      </c>
+      <c r="D5" s="1">
+        <f>A5*L5%</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f>A5*M5%</f>
+        <v>12.978000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5*N5%</f>
+        <v>2.016</v>
+      </c>
+      <c r="G5" s="1">
+        <f>A5*O5%</f>
+        <v>26.018999999999998</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <v>23.8</v>
+      </c>
+      <c r="K5">
+        <v>11.1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>20.6</v>
+      </c>
+      <c r="N5">
+        <v>3.2</v>
+      </c>
+      <c r="O5">
+        <v>41.3</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <f>(100-89.5)/2</f>
+        <v>5.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Done with first preference
</commit_message>
<xml_diff>
--- a/static/excel/IDC.xlsx
+++ b/static/excel/IDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit\Documents\IDC\decisionmaker\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6A1566-0BF1-4E15-BD62-14E6ABD96F5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B5CA32-4F0E-4BC2-8379-8311A81C3FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIP" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="21">
   <si>
     <t>1st Pref</t>
   </si>
@@ -100,15 +100,6 @@
   </si>
   <si>
     <t>ACN</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -1581,7 +1572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6ECE78-ECAB-4BF0-A9D2-F1C8D49456BF}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:P5"/>
     </sheetView>
   </sheetViews>
@@ -2151,10 +2142,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A16B396-E65E-4B47-B1DE-118E1660A500}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,12 +2421,6 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="O9">
-        <f>(100-89.5)/2</f>
-        <v>5.25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new record and cleared some data
</commit_message>
<xml_diff>
--- a/static/excel/IDC.xlsx
+++ b/static/excel/IDC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit\Documents\Electives\decisionmaker\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED48D45-086F-4BDA-92CC-3AC3E5CEFB89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9E631C-E90A-475D-932C-D60C7A2B6E29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,277 +815,167 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" ref="B8" si="11">A8*J8%</f>
-        <v>10.974</v>
+        <v>10.989000000000001</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" ref="C8" si="12">A8*K8%</f>
-        <v>10.044</v>
+        <v>9.9989999999999988</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" ref="D8" si="13">A8*L8%</f>
-        <v>30.968999999999998</v>
+        <v>31.976999999999997</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" ref="E8" si="14">A8*M8%</f>
-        <v>14.973000000000001</v>
+        <v>16.038</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" ref="F8" si="15">A8*N8%</f>
-        <v>9.020999999999999</v>
+        <v>12.969000000000001</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" ref="G8" si="16">A8*O8%</f>
-        <v>14.973000000000001</v>
+        <v>15.048</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" ref="H8" si="17">SUM(B8:G8)</f>
-        <v>90.953999999999994</v>
+        <v>97.02000000000001</v>
       </c>
       <c r="J8">
-        <v>11.8</v>
+        <v>11.1</v>
       </c>
       <c r="K8">
-        <v>10.8</v>
+        <v>10.1</v>
       </c>
       <c r="L8">
-        <v>33.299999999999997</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="M8">
-        <v>16.100000000000001</v>
+        <v>16.2</v>
       </c>
       <c r="N8">
-        <v>9.6999999999999993</v>
+        <v>13.1</v>
       </c>
       <c r="O8">
-        <v>16.100000000000001</v>
+        <v>15.2</v>
       </c>
       <c r="P8">
         <f t="shared" ref="P8" si="18">SUM(J8:O8)</f>
-        <v>97.800000000000011</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" ref="B9" si="19">A9*J9%</f>
-        <v>10.989000000000001</v>
+        <f t="shared" ref="B9:B10" si="19">A9*J9%</f>
+        <v>12.98</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" ref="C9" si="20">A9*K9%</f>
-        <v>9.9989999999999988</v>
+        <f t="shared" ref="C9:C10" si="20">A9*K9%</f>
+        <v>11</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" ref="D9" si="21">A9*L9%</f>
-        <v>31.976999999999997</v>
+        <f t="shared" ref="D9:D10" si="21">A9*L9%</f>
+        <v>36.96</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ref="E9" si="22">A9*M9%</f>
-        <v>16.038</v>
+        <f t="shared" ref="E9:E10" si="22">A9*M9%</f>
+        <v>19.03</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" ref="F9" si="23">A9*N9%</f>
-        <v>12.969000000000001</v>
+        <f t="shared" ref="F9:F10" si="23">A9*N9%</f>
+        <v>12.98</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" ref="G9" si="24">A9*O9%</f>
-        <v>15.048</v>
+        <f t="shared" ref="G9:G10" si="24">A9*O9%</f>
+        <v>14.96</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" ref="H9" si="25">SUM(B9:G9)</f>
-        <v>97.02000000000001</v>
+        <f t="shared" ref="H9:H10" si="25">SUM(B9:G9)</f>
+        <v>107.91</v>
       </c>
       <c r="J9">
-        <v>11.1</v>
+        <v>11.8</v>
       </c>
       <c r="K9">
-        <v>10.1</v>
+        <v>10</v>
       </c>
       <c r="L9">
-        <v>32.299999999999997</v>
+        <v>33.6</v>
       </c>
       <c r="M9">
-        <v>16.2</v>
+        <v>17.3</v>
       </c>
       <c r="N9">
-        <v>13.1</v>
+        <v>11.8</v>
       </c>
       <c r="O9">
-        <v>15.2</v>
+        <v>13.6</v>
       </c>
       <c r="P9">
-        <f t="shared" ref="P9" si="26">SUM(J9:O9)</f>
-        <v>98</v>
+        <f t="shared" ref="P9:P10" si="26">SUM(J9:O9)</f>
+        <v>98.1</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" ref="B10" si="27">A10*J10%</f>
-        <v>11.020999999999999</v>
+        <f t="shared" si="19"/>
+        <v>19.019000000000002</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" ref="C10" si="28">A10*K10%</f>
-        <v>9.9909999999999997</v>
+        <f t="shared" si="20"/>
+        <v>15.959999999999999</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" ref="D10" si="29">A10*L10%</f>
-        <v>33.99</v>
+        <f t="shared" si="21"/>
+        <v>46.018000000000001</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" ref="E10" si="30">A10*M10%</f>
-        <v>18.024999999999999</v>
+        <f t="shared" si="22"/>
+        <v>21.013999999999999</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" ref="F10" si="31">A10*N10%</f>
-        <v>12.978</v>
+        <f t="shared" si="23"/>
+        <v>13.965</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" ref="G10" si="32">A10*O10%</f>
-        <v>15.037999999999998</v>
+        <f t="shared" si="24"/>
+        <v>15.029</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" ref="H10" si="33">SUM(B10:G10)</f>
-        <v>101.04299999999999</v>
+        <f t="shared" si="25"/>
+        <v>131.005</v>
       </c>
       <c r="J10">
-        <v>10.7</v>
+        <v>14.3</v>
       </c>
       <c r="K10">
-        <v>9.6999999999999993</v>
+        <v>12</v>
       </c>
       <c r="L10">
-        <v>33</v>
+        <v>34.6</v>
       </c>
       <c r="M10">
-        <v>17.5</v>
+        <v>15.8</v>
       </c>
       <c r="N10">
-        <v>12.6</v>
+        <v>10.5</v>
       </c>
       <c r="O10">
-        <v>14.6</v>
+        <v>11.3</v>
       </c>
       <c r="P10">
-        <f t="shared" ref="P10" si="34">SUM(J10:O10)</f>
-        <v>98.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>108</v>
-      </c>
-      <c r="B11" s="1">
-        <f t="shared" ref="B11" si="35">A11*J11%</f>
-        <v>12.959999999999999</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" ref="C11" si="36">A11*K11%</f>
-        <v>11.016</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" ref="D11" si="37">A11*L11%</f>
-        <v>35.963999999999999</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" ref="E11" si="38">A11*M11%</f>
-        <v>18.035999999999998</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" ref="F11" si="39">A11*N11%</f>
-        <v>12.959999999999999</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" ref="G11" si="40">A11*O11%</f>
-        <v>15.012</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" ref="H11" si="41">SUM(B11:G11)</f>
-        <v>105.94799999999999</v>
-      </c>
-      <c r="J11">
-        <v>12</v>
-      </c>
-      <c r="K11">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="L11">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="M11">
-        <v>16.7</v>
-      </c>
-      <c r="N11">
-        <v>12</v>
-      </c>
-      <c r="O11">
-        <v>13.9</v>
-      </c>
-      <c r="P11">
-        <f t="shared" ref="P11" si="42">SUM(J11:O11)</f>
-        <v>98.100000000000009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>110</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" ref="B12" si="43">A12*J12%</f>
-        <v>12.98</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" ref="C12" si="44">A12*K12%</f>
-        <v>11</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" ref="D12" si="45">A12*L12%</f>
-        <v>36.96</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" ref="E12" si="46">A12*M12%</f>
-        <v>19.03</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" ref="F12" si="47">A12*N12%</f>
-        <v>12.98</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" ref="G12" si="48">A12*O12%</f>
-        <v>14.96</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" ref="H12" si="49">SUM(B12:G12)</f>
-        <v>107.91</v>
-      </c>
-      <c r="J12">
-        <v>11.8</v>
-      </c>
-      <c r="K12">
-        <v>10</v>
-      </c>
-      <c r="L12">
-        <v>33.6</v>
-      </c>
-      <c r="M12">
-        <v>17.3</v>
-      </c>
-      <c r="N12">
-        <v>11.8</v>
-      </c>
-      <c r="O12">
-        <v>13.6</v>
-      </c>
-      <c r="P12">
-        <f t="shared" ref="P12" si="50">SUM(J12:O12)</f>
-        <v>98.1</v>
+        <f t="shared" si="26"/>
+        <v>98.5</v>
       </c>
     </row>
   </sheetData>
@@ -1095,10 +985,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312D2B4B-65DA-4A16-B682-41207C4E444E}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="A9" sqref="A9:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,96 +1379,96 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ref="B8:B12" si="10">A8*J8%</f>
-        <v>10.974</v>
+        <f t="shared" ref="B8:B10" si="10">A8*J8%</f>
+        <v>10.989000000000001</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C12" si="11">A8*K8%</f>
-        <v>5.0220000000000002</v>
+        <f t="shared" ref="C8:C10" si="11">A8*K8%</f>
+        <v>5.0489999999999995</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8:D12" si="12">A8*L8%</f>
-        <v>62.031000000000006</v>
+        <f t="shared" ref="D8:D10" si="12">A8*L8%</f>
+        <v>62.963999999999999</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ref="E8:E9" si="13">A8*M8%</f>
+        <f t="shared" ref="E8" si="13">A8*M8%</f>
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8:F9" si="14">A8*N8%</f>
-        <v>11.997</v>
+        <f t="shared" ref="F8" si="14">A8*N8%</f>
+        <v>17.027999999999999</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G9" si="15">A8*O8%</f>
-        <v>2.976</v>
+        <f t="shared" ref="G8" si="15">A8*O8%</f>
+        <v>2.9699999999999998</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" ref="H8:H12" si="16">SUM(B8:G8)</f>
-        <v>93</v>
+        <f t="shared" ref="H8:H10" si="16">SUM(B8:G8)</f>
+        <v>99</v>
       </c>
       <c r="J8">
-        <v>11.8</v>
+        <v>11.1</v>
       </c>
       <c r="K8">
-        <v>5.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="L8">
-        <v>66.7</v>
+        <v>63.6</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>12.9</v>
+        <v>17.2</v>
       </c>
       <c r="O8">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:P9" si="17">SUM(J8:O8)</f>
-        <v>100.00000000000001</v>
+        <f t="shared" ref="P8" si="17">SUM(J8:O8)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="10"/>
-        <v>10.989000000000001</v>
+        <v>12.98</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="11"/>
-        <v>5.0489999999999995</v>
+        <v>6.05</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="12"/>
-        <v>62.963999999999999</v>
+        <v>69.960000000000008</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="E9:E10" si="18">A9*M9%</f>
         <v>0</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="14"/>
-        <v>17.027999999999999</v>
+        <f t="shared" ref="F9:F10" si="19">A9*N9%</f>
+        <v>18.04</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="15"/>
-        <v>2.9699999999999998</v>
+        <f t="shared" ref="G9:G10" si="20">A9*O9%</f>
+        <v>2.97</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="16"/>
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="J9">
-        <v>11.1</v>
+        <v>11.8</v>
       </c>
       <c r="K9">
-        <v>5.0999999999999996</v>
+        <v>5.5</v>
       </c>
       <c r="L9">
         <v>63.6</v>
@@ -1587,56 +1477,56 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>17.2</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="O9">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="P9">
-        <f t="shared" si="17"/>
-        <v>100</v>
+        <f t="shared" ref="P9:P10" si="21">SUM(J9:O9)</f>
+        <v>100.00000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="10"/>
-        <v>11.020999999999999</v>
+        <v>19.019000000000002</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="11"/>
-        <v>5.9739999999999993</v>
+        <v>5.9849999999999994</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="12"/>
-        <v>66.022999999999996</v>
+        <v>82.992000000000004</v>
       </c>
       <c r="E10" s="1">
-        <f>A10*M10%</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <f>A10*N10%</f>
-        <v>16.995000000000001</v>
+        <f t="shared" si="19"/>
+        <v>21.945</v>
       </c>
       <c r="G10" s="1">
-        <f>A10*O10%</f>
-        <v>2.9869999999999997</v>
+        <f t="shared" si="20"/>
+        <v>3.0590000000000002</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="16"/>
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="J10">
-        <v>10.7</v>
+        <v>14.3</v>
       </c>
       <c r="K10">
-        <v>5.8</v>
+        <v>4.5</v>
       </c>
       <c r="L10">
-        <v>64.099999999999994</v>
+        <v>62.4</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1645,121 +1535,11 @@
         <v>16.5</v>
       </c>
       <c r="O10">
-        <v>2.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="P10">
-        <f>SUM(J10:O10)</f>
+        <f t="shared" si="21"/>
         <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>108</v>
-      </c>
-      <c r="B11" s="1">
-        <f t="shared" si="10"/>
-        <v>12.959999999999999</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" si="11"/>
-        <v>6.0479999999999992</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" si="12"/>
-        <v>69.012</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" ref="E11:E12" si="18">A11*M11%</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" ref="F11:F12" si="19">A11*N11%</f>
-        <v>16.956</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" ref="G11:G12" si="20">A11*O11%</f>
-        <v>3.0239999999999996</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" si="16"/>
-        <v>108</v>
-      </c>
-      <c r="J11">
-        <v>12</v>
-      </c>
-      <c r="K11">
-        <v>5.6</v>
-      </c>
-      <c r="L11">
-        <v>63.9</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>15.7</v>
-      </c>
-      <c r="O11">
-        <v>2.8</v>
-      </c>
-      <c r="P11">
-        <f t="shared" ref="P11:P12" si="21">SUM(J11:O11)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>110</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" si="10"/>
-        <v>12.98</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="11"/>
-        <v>6.05</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="12"/>
-        <v>69.960000000000008</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="19"/>
-        <v>18.04</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="20"/>
-        <v>2.97</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="16"/>
-        <v>110</v>
-      </c>
-      <c r="J12">
-        <v>11.8</v>
-      </c>
-      <c r="K12">
-        <v>5.5</v>
-      </c>
-      <c r="L12">
-        <v>63.6</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="O12">
-        <v>2.7</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="21"/>
-        <v>100.00000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1769,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE7E77F-95DD-4B10-83E4-041B3BBF5D3C}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,277 +1940,167 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ref="B8" si="11">A8*J8%</f>
-        <v>10.044</v>
+        <f t="shared" ref="B8:B10" si="11">A8*J8%</f>
+        <v>9.9989999999999988</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8" si="12">A8*K8%</f>
-        <v>10.974</v>
+        <f t="shared" ref="C8:C10" si="12">A8*K8%</f>
+        <v>10.989000000000001</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8" si="13">A8*L8%</f>
-        <v>14.042999999999999</v>
+        <f t="shared" ref="D8:D10" si="13">A8*L8%</f>
+        <v>19.007999999999999</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ref="E8" si="14">A8*M8%</f>
+        <f t="shared" ref="E8:E10" si="14">A8*M8%</f>
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8" si="15">A8*N8%</f>
-        <v>51.986999999999995</v>
+        <f t="shared" ref="F8:F10" si="15">A8*N8%</f>
+        <v>52.965000000000003</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8" si="16">A8*O8%</f>
-        <v>6.0449999999999999</v>
+        <f t="shared" ref="G8:G10" si="16">A8*O8%</f>
+        <v>6.0389999999999997</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" ref="H8" si="17">SUM(B8:G8)</f>
-        <v>93.093000000000004</v>
+        <f t="shared" ref="H8:H10" si="17">SUM(B8:G8)</f>
+        <v>99</v>
       </c>
       <c r="J8">
-        <v>10.8</v>
+        <v>10.1</v>
       </c>
       <c r="K8">
-        <v>11.8</v>
+        <v>11.1</v>
       </c>
       <c r="L8">
-        <v>15.1</v>
+        <v>19.2</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>55.9</v>
+        <v>53.5</v>
       </c>
       <c r="O8">
-        <v>6.5</v>
+        <v>6.1</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8" si="18">SUM(J8:O8)</f>
-        <v>100.1</v>
+        <f t="shared" ref="P8:P10" si="18">SUM(J8:O8)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" ref="B9:B12" si="19">A9*J9%</f>
-        <v>9.9989999999999988</v>
+        <f t="shared" si="11"/>
+        <v>11</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" ref="C9:C12" si="20">A9*K9%</f>
-        <v>10.989000000000001</v>
+        <f t="shared" si="12"/>
+        <v>12.98</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" ref="D9:D12" si="21">A9*L9%</f>
-        <v>19.007999999999999</v>
+        <f t="shared" si="13"/>
+        <v>20.02</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ref="E9:E12" si="22">A9*M9%</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" ref="F9:F12" si="23">A9*N9%</f>
-        <v>52.965000000000003</v>
+        <f t="shared" si="15"/>
+        <v>57.970000000000006</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" ref="G9:G12" si="24">A9*O9%</f>
-        <v>6.0389999999999997</v>
+        <f t="shared" si="16"/>
+        <v>8.0299999999999994</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" ref="H9:H12" si="25">SUM(B9:G9)</f>
-        <v>99</v>
+        <f t="shared" si="17"/>
+        <v>110</v>
       </c>
       <c r="J9">
-        <v>10.1</v>
-      </c>
-      <c r="K9">
-        <v>11.1</v>
+        <v>10</v>
+      </c>
+      <c r="K9" s="3">
+        <v>11.8</v>
       </c>
       <c r="L9">
-        <v>19.2</v>
+        <v>18.2</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>53.5</v>
+        <v>52.7</v>
       </c>
       <c r="O9">
-        <v>6.1</v>
+        <v>7.3</v>
       </c>
       <c r="P9">
-        <f t="shared" ref="P9:P12" si="26">SUM(J9:O9)</f>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="19"/>
-        <v>9.9909999999999997</v>
+        <f t="shared" si="11"/>
+        <v>15.959999999999999</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="20"/>
-        <v>12.050999999999998</v>
+        <f t="shared" si="12"/>
+        <v>15.029</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="21"/>
-        <v>18.951999999999998</v>
+        <f t="shared" si="13"/>
+        <v>23.939999999999998</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="23"/>
-        <v>55.002000000000002</v>
+        <f t="shared" si="15"/>
+        <v>69.957999999999998</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="24"/>
-        <v>7.0040000000000004</v>
+        <f t="shared" si="16"/>
+        <v>7.9799999999999995</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="25"/>
-        <v>103.00000000000001</v>
+        <f t="shared" si="17"/>
+        <v>132.86699999999999</v>
       </c>
       <c r="J10">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="K10">
-        <v>11.7</v>
+        <v>12</v>
+      </c>
+      <c r="K10" s="3">
+        <v>11.3</v>
       </c>
       <c r="L10">
-        <v>18.399999999999999</v>
+        <v>18</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>53.4</v>
+        <v>52.6</v>
       </c>
       <c r="O10">
-        <v>6.8</v>
+        <v>6</v>
       </c>
       <c r="P10">
-        <f t="shared" si="26"/>
-        <v>99.999999999999986</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>108</v>
-      </c>
-      <c r="B11" s="1">
-        <f t="shared" si="19"/>
-        <v>11.016</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" si="20"/>
-        <v>12.959999999999999</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" si="21"/>
-        <v>19.008000000000003</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="23"/>
-        <v>57.024000000000001</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" si="24"/>
-        <v>7.9920000000000009</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" si="25"/>
-        <v>108.00000000000001</v>
-      </c>
-      <c r="J11">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="K11">
-        <v>12</v>
-      </c>
-      <c r="L11">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>52.8</v>
-      </c>
-      <c r="O11">
-        <v>7.4</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="26"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>110</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" si="19"/>
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="20"/>
-        <v>12.98</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="21"/>
-        <v>20.02</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="23"/>
-        <v>57.970000000000006</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="24"/>
-        <v>8.0299999999999994</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="25"/>
-        <v>110</v>
-      </c>
-      <c r="J12">
-        <v>10</v>
-      </c>
-      <c r="K12" s="3">
-        <v>11.8</v>
-      </c>
-      <c r="L12">
-        <v>18.2</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>52.7</v>
-      </c>
-      <c r="O12">
-        <v>7.3</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="26"/>
-        <v>100</v>
+        <f t="shared" si="18"/>
+        <v>99.9</v>
       </c>
     </row>
   </sheetData>
@@ -2440,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59225AD-4E49-4CB8-BC4D-705EABA206D1}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2833,109 +2503,108 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ref="B8:B12" si="12">A8*J8%</f>
-        <v>30.968999999999998</v>
+        <f t="shared" ref="B8:B10" si="12">A8*J8%</f>
+        <v>31.976999999999997</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C12" si="13">A8*K8%</f>
-        <v>10.974</v>
+        <f t="shared" ref="C8:C10" si="13">A8*K8%</f>
+        <v>16.038</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8:D12" si="14">A8*L8%</f>
-        <v>9.020999999999999</v>
+        <f t="shared" ref="D8:D10" si="14">A8*L8%</f>
+        <v>9.0090000000000003</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ref="E8:E12" si="15">A8*M8%</f>
-        <v>17.018999999999998</v>
+        <f t="shared" ref="E8:E10" si="15">A8*M8%</f>
+        <v>17.027999999999999</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8:F12" si="16">A8*N8%</f>
-        <v>17.018999999999998</v>
+        <f t="shared" ref="F8:F10" si="16">A8*N8%</f>
+        <v>17.027999999999999</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G12" si="17">A8*O8%</f>
-        <v>7.9979999999999993</v>
+        <f t="shared" ref="G8:G10" si="17">A8*O8%</f>
+        <v>8.0190000000000001</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" ref="H8:H12" si="18">SUM(B8:G8)</f>
-        <v>93.000000000000014</v>
-      </c>
-      <c r="I8" s="1"/>
+        <f t="shared" ref="H8:H10" si="18">SUM(B8:G8)</f>
+        <v>99.09899999999999</v>
+      </c>
       <c r="J8">
-        <v>33.299999999999997</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="K8">
-        <v>11.8</v>
+        <v>16.2</v>
       </c>
       <c r="L8">
-        <v>9.6999999999999993</v>
+        <v>9.1</v>
       </c>
       <c r="M8">
-        <v>18.3</v>
+        <v>17.2</v>
       </c>
       <c r="N8">
-        <v>18.3</v>
+        <v>17.2</v>
       </c>
       <c r="O8">
-        <v>8.6</v>
+        <v>8.1</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:P12" si="19">SUM(J8:O8)</f>
-        <v>99.999999999999986</v>
+        <f t="shared" ref="P8:P10" si="19">SUM(J8:O8)</f>
+        <v>100.1</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="12"/>
-        <v>31.976999999999997</v>
+        <v>36.96</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="13"/>
-        <v>16.038</v>
+        <v>18.04</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="14"/>
-        <v>9.0090000000000003</v>
+        <v>10.01</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="15"/>
-        <v>17.027999999999999</v>
+        <v>17.05</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="16"/>
-        <v>17.027999999999999</v>
+        <v>20.02</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="17"/>
-        <v>8.0190000000000001</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="18"/>
-        <v>99.09899999999999</v>
+        <v>110.11</v>
       </c>
       <c r="J9">
-        <v>32.299999999999997</v>
+        <v>33.6</v>
       </c>
       <c r="K9">
-        <v>16.2</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="L9">
         <v>9.1</v>
       </c>
       <c r="M9">
-        <v>17.2</v>
+        <v>15.5</v>
       </c>
       <c r="N9">
-        <v>17.2</v>
+        <v>18.2</v>
       </c>
       <c r="O9">
-        <v>8.1</v>
+        <v>7.3</v>
       </c>
       <c r="P9">
         <f t="shared" si="19"/>
@@ -2944,167 +2613,57 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="12"/>
-        <v>33.99</v>
+        <v>46.018000000000001</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="13"/>
-        <v>16.995000000000001</v>
+        <v>21.945</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="14"/>
-        <v>8.9609999999999985</v>
+        <v>13.965</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="15"/>
-        <v>16.995000000000001</v>
+        <v>17.955000000000002</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="16"/>
-        <v>18.024999999999999</v>
+        <v>23.939999999999998</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="17"/>
-        <v>8.0340000000000007</v>
+        <v>9.0440000000000005</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="18"/>
-        <v>103.00000000000001</v>
+        <v>132.86699999999999</v>
       </c>
       <c r="J10">
-        <v>33</v>
+        <v>34.6</v>
       </c>
       <c r="K10">
         <v>16.5</v>
       </c>
       <c r="L10">
-        <v>8.6999999999999993</v>
+        <v>10.5</v>
       </c>
       <c r="M10">
-        <v>16.5</v>
+        <v>13.5</v>
       </c>
       <c r="N10">
-        <v>17.5</v>
+        <v>18</v>
       </c>
       <c r="O10">
-        <v>7.8</v>
+        <v>6.8</v>
       </c>
       <c r="P10">
         <f t="shared" si="19"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>108</v>
-      </c>
-      <c r="B11" s="1">
-        <f t="shared" si="12"/>
-        <v>35.963999999999999</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" si="13"/>
-        <v>16.956</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" si="14"/>
-        <v>10.044000000000002</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="15"/>
-        <v>16.956</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="16"/>
-        <v>19.98</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" si="17"/>
-        <v>7.9920000000000009</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" si="18"/>
-        <v>107.89200000000001</v>
-      </c>
-      <c r="J11">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="K11">
-        <v>15.7</v>
-      </c>
-      <c r="L11">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="M11">
-        <v>15.7</v>
-      </c>
-      <c r="N11">
-        <v>18.5</v>
-      </c>
-      <c r="O11">
-        <v>7.4</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="19"/>
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>110</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" si="12"/>
-        <v>36.96</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="13"/>
-        <v>18.04</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="14"/>
-        <v>10.01</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="15"/>
-        <v>17.05</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="16"/>
-        <v>20.02</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="17"/>
-        <v>8.0299999999999994</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="18"/>
-        <v>110.11</v>
-      </c>
-      <c r="J12">
-        <v>33.6</v>
-      </c>
-      <c r="K12">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="L12">
-        <v>9.1</v>
-      </c>
-      <c r="M12">
-        <v>15.5</v>
-      </c>
-      <c r="N12">
-        <v>18.2</v>
-      </c>
-      <c r="O12">
-        <v>7.3</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="19"/>
-        <v>100.1</v>
+        <v>99.899999999999991</v>
       </c>
     </row>
   </sheetData>
@@ -3114,10 +2673,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6ECE78-ECAB-4BF0-A9D2-F1C8D49456BF}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="A9" sqref="A9:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3507,278 +3066,167 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ref="B8:B12" si="12">A8*J8%</f>
-        <v>14.973000000000001</v>
+        <f t="shared" ref="B8:B10" si="12">A8*J8%</f>
+        <v>16.038</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C12" si="13">A8*K8%</f>
-        <v>26.040000000000003</v>
+        <f t="shared" ref="C8:C10" si="13">A8*K8%</f>
+        <v>26.037000000000003</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8:D12" si="14">A8*L8%</f>
-        <v>5.0220000000000002</v>
+        <f t="shared" ref="D8:D10" si="14">A8*L8%</f>
+        <v>5.0489999999999995</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ref="E8:E12" si="15">A8*M8%</f>
-        <v>34.037999999999997</v>
+        <f t="shared" ref="E8:E10" si="15">A8*M8%</f>
+        <v>35.045999999999999</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8:F12" si="16">A8*N8%</f>
-        <v>9.020999999999999</v>
+        <f t="shared" ref="F8:F10" si="16">A8*N8%</f>
+        <v>9.0090000000000003</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G12" si="17">A8*O8%</f>
-        <v>3.9989999999999997</v>
+        <f t="shared" ref="G8:G10" si="17">A8*O8%</f>
+        <v>8.0190000000000001</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" ref="H8:H12" si="18">SUM(B8:G8)</f>
-        <v>93.093000000000004</v>
-      </c>
-      <c r="I8" s="1"/>
+        <f t="shared" ref="H8:H10" si="18">SUM(B8:G8)</f>
+        <v>99.198000000000008</v>
+      </c>
       <c r="J8">
-        <v>16.100000000000001</v>
+        <v>16.2</v>
       </c>
       <c r="K8">
-        <v>28</v>
+        <v>26.3</v>
       </c>
       <c r="L8">
-        <v>5.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="M8">
-        <v>36.6</v>
+        <v>35.4</v>
       </c>
       <c r="N8">
-        <v>9.6999999999999993</v>
+        <v>9.1</v>
       </c>
       <c r="O8">
-        <v>4.3</v>
+        <v>8.1</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:P12" si="19">SUM(J8:O8)</f>
-        <v>100.1</v>
+        <f t="shared" ref="P8:P10" si="19">SUM(J8:O8)</f>
+        <v>100.19999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="12"/>
-        <v>16.038</v>
+        <v>19.03</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="13"/>
-        <v>26.037000000000003</v>
+        <v>28.05</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="14"/>
-        <v>5.0489999999999995</v>
+        <v>6.05</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="15"/>
-        <v>35.045999999999999</v>
+        <v>36.96</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="16"/>
-        <v>9.0090000000000003</v>
+        <v>10.01</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="17"/>
-        <v>8.0190000000000001</v>
+        <v>10.01</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="18"/>
-        <v>99.198000000000008</v>
+        <v>110.11000000000001</v>
       </c>
       <c r="J9">
-        <v>16.2</v>
+        <v>17.3</v>
       </c>
       <c r="K9">
-        <v>26.3</v>
+        <v>25.5</v>
       </c>
       <c r="L9">
-        <v>5.0999999999999996</v>
+        <v>5.5</v>
       </c>
       <c r="M9">
-        <v>35.4</v>
+        <v>33.6</v>
       </c>
       <c r="N9">
         <v>9.1</v>
       </c>
       <c r="O9">
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
       <c r="P9">
         <f t="shared" si="19"/>
-        <v>100.19999999999999</v>
+        <v>100.1</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="12"/>
-        <v>18.024999999999999</v>
+        <v>21.013999999999999</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="13"/>
-        <v>26.986000000000001</v>
+        <v>34.978999999999999</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="14"/>
-        <v>5.9739999999999993</v>
+        <v>7.0489999999999995</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="15"/>
-        <v>35.020000000000003</v>
+        <v>44.953999999999994</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="16"/>
-        <v>8.9609999999999985</v>
+        <v>11.969999999999999</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="17"/>
-        <v>8.0340000000000007</v>
+        <v>13.034000000000001</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="18"/>
-        <v>103</v>
+        <v>132.99999999999997</v>
       </c>
       <c r="J10">
-        <v>17.5</v>
+        <v>15.8</v>
       </c>
       <c r="K10">
-        <v>26.2</v>
+        <v>26.3</v>
       </c>
       <c r="L10">
-        <v>5.8</v>
+        <v>5.3</v>
       </c>
       <c r="M10">
-        <v>34</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="N10">
-        <v>8.6999999999999993</v>
+        <v>9</v>
       </c>
       <c r="O10">
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="P10">
         <f t="shared" si="19"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>108</v>
-      </c>
-      <c r="B11" s="1">
-        <f t="shared" si="12"/>
-        <v>18.035999999999998</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" si="13"/>
-        <v>27.972000000000001</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" si="14"/>
-        <v>6.0479999999999992</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="15"/>
-        <v>35.963999999999999</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="16"/>
-        <v>10.044000000000002</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" si="17"/>
-        <v>10.044000000000002</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" si="18"/>
-        <v>108.10799999999999</v>
-      </c>
-      <c r="J11">
-        <v>16.7</v>
-      </c>
-      <c r="K11">
-        <v>25.9</v>
-      </c>
-      <c r="L11">
-        <v>5.6</v>
-      </c>
-      <c r="M11">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="N11">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="O11">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="19"/>
-        <v>100.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>110</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" si="12"/>
-        <v>19.03</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="13"/>
-        <v>28.05</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="14"/>
-        <v>6.05</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="15"/>
-        <v>36.96</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="16"/>
-        <v>10.01</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="17"/>
-        <v>10.01</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="18"/>
-        <v>110.11000000000001</v>
-      </c>
-      <c r="J12">
-        <v>17.3</v>
-      </c>
-      <c r="K12">
-        <v>25.5</v>
-      </c>
-      <c r="L12">
-        <v>5.5</v>
-      </c>
-      <c r="M12">
-        <v>33.6</v>
-      </c>
-      <c r="N12">
-        <v>9.1</v>
-      </c>
-      <c r="O12">
-        <v>9.1</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="19"/>
-        <v>100.1</v>
+        <v>99.999999999999986</v>
       </c>
     </row>
   </sheetData>
@@ -3788,10 +3236,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF3A003-6591-43A0-AC06-C46B170D979B}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="A9" sqref="A9:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4181,278 +3629,167 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ref="B8:B12" si="11">A8*J8%</f>
-        <v>9.020999999999999</v>
+        <f t="shared" ref="B8:B10" si="11">A8*J8%</f>
+        <v>12.969000000000001</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C12" si="12">A8*K8%</f>
-        <v>22.041</v>
+        <f t="shared" ref="C8:C10" si="12">A8*K8%</f>
+        <v>22.968</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8:D12" si="13">A8*L8%</f>
-        <v>6.0449999999999999</v>
+        <f t="shared" ref="D8:D10" si="13">A8*L8%</f>
+        <v>6.0389999999999997</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ref="E8:E12" si="14">A8*M8%</f>
-        <v>22.041</v>
+        <f t="shared" ref="E8:E10" si="14">A8*M8%</f>
+        <v>22.968</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8:F12" si="15">A8*N8%</f>
-        <v>1.0230000000000001</v>
+        <f t="shared" ref="F8:F10" si="15">A8*N8%</f>
+        <v>1.0890000000000002</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G12" si="16">A8*O8%</f>
-        <v>33.015000000000001</v>
+        <f t="shared" ref="G8:G10" si="16">A8*O8%</f>
+        <v>32.966999999999999</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" ref="H8:H12" si="17">SUM(B8:G8)</f>
-        <v>93.186000000000007</v>
-      </c>
-      <c r="I8" s="1"/>
+        <f t="shared" ref="H8:H10" si="17">SUM(B8:G8)</f>
+        <v>99</v>
+      </c>
       <c r="J8">
-        <v>9.6999999999999993</v>
+        <v>13.1</v>
       </c>
       <c r="K8">
-        <v>23.7</v>
+        <v>23.2</v>
       </c>
       <c r="L8">
-        <v>6.5</v>
+        <v>6.1</v>
       </c>
       <c r="M8">
-        <v>23.7</v>
+        <v>23.2</v>
       </c>
       <c r="N8">
         <v>1.1000000000000001</v>
       </c>
       <c r="O8">
-        <v>35.5</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:P12" si="18">SUM(J8:O8)</f>
-        <v>100.19999999999999</v>
+        <f t="shared" ref="P8:P10" si="18">SUM(J8:O8)</f>
+        <v>99.999999999999986</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="11"/>
-        <v>12.969000000000001</v>
+        <v>12.98</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="12"/>
-        <v>22.968</v>
+        <v>26.95</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="13"/>
-        <v>6.0389999999999997</v>
+        <v>6.05</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="14"/>
-        <v>22.968</v>
+        <v>28.05</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="15"/>
-        <v>1.0890000000000002</v>
+        <v>1.9800000000000002</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="16"/>
-        <v>32.966999999999999</v>
+        <v>33.99</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="17"/>
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="J9">
-        <v>13.1</v>
+        <v>11.8</v>
       </c>
       <c r="K9">
-        <v>23.2</v>
+        <v>24.5</v>
       </c>
       <c r="L9">
-        <v>6.1</v>
+        <v>5.5</v>
       </c>
       <c r="M9">
-        <v>23.2</v>
+        <v>25.5</v>
       </c>
       <c r="N9">
-        <v>1.1000000000000001</v>
+        <v>1.8</v>
       </c>
       <c r="O9">
-        <v>33.299999999999997</v>
+        <v>30.9</v>
       </c>
       <c r="P9">
         <f t="shared" si="18"/>
-        <v>99.999999999999986</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="11"/>
-        <v>12.978</v>
+        <v>13.965</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="12"/>
-        <v>22.969000000000001</v>
+        <v>34.978999999999999</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="13"/>
-        <v>5.9739999999999993</v>
+        <v>5.9849999999999994</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="14"/>
-        <v>25.956</v>
+        <v>32.053000000000004</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="15"/>
-        <v>1.9569999999999999</v>
+        <v>3.0590000000000002</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="16"/>
-        <v>32.96</v>
+        <v>42.826000000000001</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="17"/>
-        <v>102.79399999999998</v>
+        <v>132.86699999999999</v>
       </c>
       <c r="J10">
-        <v>12.6</v>
+        <v>10.5</v>
       </c>
       <c r="K10">
-        <v>22.3</v>
+        <v>26.3</v>
       </c>
       <c r="L10">
-        <v>5.8</v>
+        <v>4.5</v>
       </c>
       <c r="M10">
-        <v>25.2</v>
+        <v>24.1</v>
       </c>
       <c r="N10">
-        <v>1.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="O10">
-        <v>32</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="P10">
         <f t="shared" si="18"/>
-        <v>99.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>108</v>
-      </c>
-      <c r="B11" s="1">
-        <f t="shared" si="11"/>
-        <v>12.959999999999999</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" si="12"/>
-        <v>26.028000000000002</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" si="13"/>
-        <v>6.0479999999999992</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="14"/>
-        <v>27</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="15"/>
-        <v>2.052</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" si="16"/>
-        <v>34.020000000000003</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" si="17"/>
-        <v>108.108</v>
-      </c>
-      <c r="J11">
-        <v>12</v>
-      </c>
-      <c r="K11">
-        <v>24.1</v>
-      </c>
-      <c r="L11">
-        <v>5.6</v>
-      </c>
-      <c r="M11">
-        <v>25</v>
-      </c>
-      <c r="N11">
-        <v>1.9</v>
-      </c>
-      <c r="O11">
-        <v>31.5</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="18"/>
-        <v>100.10000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>110</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" si="11"/>
-        <v>12.98</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="12"/>
-        <v>26.95</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="13"/>
-        <v>6.05</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="14"/>
-        <v>28.05</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="15"/>
-        <v>1.9800000000000002</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="16"/>
-        <v>33.99</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="17"/>
-        <v>110</v>
-      </c>
-      <c r="J12">
-        <v>11.8</v>
-      </c>
-      <c r="K12">
-        <v>24.5</v>
-      </c>
-      <c r="L12">
-        <v>5.5</v>
-      </c>
-      <c r="M12">
-        <v>25.5</v>
-      </c>
-      <c r="N12">
-        <v>1.8</v>
-      </c>
-      <c r="O12">
-        <v>30.9</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="18"/>
-        <v>100</v>
+        <v>99.9</v>
       </c>
     </row>
   </sheetData>
@@ -4462,10 +3799,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A16B396-E65E-4B47-B1DE-118E1660A500}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="A9" sqref="A9:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4855,278 +4192,167 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ref="B8:B12" si="12">A8*J8%</f>
-        <v>14.973000000000001</v>
+        <f t="shared" ref="B8:B9" si="12">A8*J8%</f>
+        <v>15.048</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C12" si="13">A8*K8%</f>
-        <v>18.971999999999998</v>
+        <f t="shared" ref="C8:C9" si="13">A8*K8%</f>
+        <v>19.007999999999999</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8:D12" si="14">A8*L8%</f>
-        <v>1.0230000000000001</v>
+        <f t="shared" ref="D8:D9" si="14">A8*L8%</f>
+        <v>0.99</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ref="E8:E12" si="15">A8*M8%</f>
-        <v>17.018999999999998</v>
+        <f t="shared" ref="E8:E9" si="15">A8*M8%</f>
+        <v>20.988</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8:F12" si="16">A8*N8%</f>
-        <v>2.976</v>
+        <f t="shared" ref="F8:F9" si="16">A8*N8%</f>
+        <v>2.9699999999999998</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G12" si="17">A8*O8%</f>
-        <v>38.036999999999999</v>
+        <f t="shared" ref="G8:G9" si="17">A8*O8%</f>
+        <v>39.995999999999995</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" ref="H8:H12" si="18">SUM(B8:G8)</f>
-        <v>93</v>
-      </c>
-      <c r="I8" s="1"/>
+        <f t="shared" ref="H8:H9" si="18">SUM(B8:G8)</f>
+        <v>99</v>
+      </c>
       <c r="J8">
-        <v>16.100000000000001</v>
+        <v>15.2</v>
       </c>
       <c r="K8">
-        <v>20.399999999999999</v>
+        <v>19.2</v>
       </c>
       <c r="L8">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="M8">
-        <v>18.3</v>
+        <v>21.2</v>
       </c>
       <c r="N8">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="O8">
-        <v>40.9</v>
+        <v>40.4</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8:P12" si="19">SUM(J8:O8)</f>
+        <f t="shared" ref="P8:P9" si="19">SUM(J8:O8)</f>
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="12"/>
-        <v>15.048</v>
+        <v>14.96</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="13"/>
-        <v>19.007999999999999</v>
+        <v>19.03</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="14"/>
-        <v>0.99</v>
+        <v>0.9900000000000001</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="15"/>
-        <v>20.988</v>
+        <v>24.97</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="16"/>
-        <v>2.9699999999999998</v>
+        <v>2.97</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="17"/>
-        <v>39.995999999999995</v>
+        <v>46.970000000000006</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="18"/>
-        <v>99</v>
+        <v>109.89000000000001</v>
       </c>
       <c r="J9">
-        <v>15.2</v>
+        <v>13.6</v>
       </c>
       <c r="K9">
-        <v>19.2</v>
+        <v>17.3</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="M9">
-        <v>21.2</v>
+        <v>22.7</v>
       </c>
       <c r="N9">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="O9">
-        <v>40.4</v>
+        <v>42.7</v>
       </c>
       <c r="P9">
         <f t="shared" si="19"/>
-        <v>100</v>
+        <v>99.9</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="12"/>
-        <v>15.037999999999998</v>
+        <f t="shared" ref="B10" si="20">A10*J10%</f>
+        <v>15.029</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="13"/>
-        <v>18.951999999999998</v>
+        <f t="shared" ref="C10" si="21">A10*K10%</f>
+        <v>21.013999999999999</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="14"/>
-        <v>1.03</v>
+        <f t="shared" ref="D10" si="22">A10*L10%</f>
+        <v>1.9949999999999999</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="15"/>
-        <v>22.041999999999998</v>
+        <f t="shared" ref="E10" si="23">A10*M10%</f>
+        <v>34.978999999999999</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="16"/>
-        <v>2.9869999999999997</v>
+        <f t="shared" ref="F10" si="24">A10*N10%</f>
+        <v>3.0590000000000002</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="17"/>
-        <v>42.951000000000001</v>
+        <f t="shared" ref="G10" si="25">A10*O10%</f>
+        <v>57.057000000000002</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="18"/>
-        <v>103</v>
+        <f t="shared" ref="H10" si="26">SUM(B10:G10)</f>
+        <v>133.13299999999998</v>
       </c>
       <c r="J10">
-        <v>14.6</v>
+        <v>11.3</v>
       </c>
       <c r="K10">
-        <v>18.399999999999999</v>
+        <v>15.8</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M10">
-        <v>21.4</v>
+        <v>26.3</v>
       </c>
       <c r="N10">
-        <v>2.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="O10">
-        <v>41.7</v>
+        <v>42.9</v>
       </c>
       <c r="P10">
-        <f t="shared" si="19"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>108</v>
-      </c>
-      <c r="B11" s="1">
-        <f t="shared" si="12"/>
-        <v>15.012</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" si="13"/>
-        <v>19.008000000000003</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" si="14"/>
-        <v>0.97200000000000009</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="15"/>
-        <v>24.948</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="16"/>
-        <v>3.0239999999999996</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" si="17"/>
-        <v>45.036000000000001</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" si="18"/>
-        <v>108</v>
-      </c>
-      <c r="J11">
-        <v>13.9</v>
-      </c>
-      <c r="K11">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="L11">
-        <v>0.9</v>
-      </c>
-      <c r="M11">
-        <v>23.1</v>
-      </c>
-      <c r="N11">
-        <v>2.8</v>
-      </c>
-      <c r="O11">
-        <v>41.7</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="19"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>110</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" si="12"/>
-        <v>14.96</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="13"/>
-        <v>19.03</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="14"/>
-        <v>0.9900000000000001</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="15"/>
-        <v>24.97</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="16"/>
-        <v>2.97</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="17"/>
-        <v>46.970000000000006</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="18"/>
-        <v>109.89000000000001</v>
-      </c>
-      <c r="J12">
-        <v>13.6</v>
-      </c>
-      <c r="K12">
-        <v>17.3</v>
-      </c>
-      <c r="L12">
-        <v>0.9</v>
-      </c>
-      <c r="M12">
-        <v>22.7</v>
-      </c>
-      <c r="N12">
-        <v>2.7</v>
-      </c>
-      <c r="O12">
-        <v>42.7</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="19"/>
-        <v>99.9</v>
+        <f t="shared" ref="P10" si="27">SUM(J10:O10)</f>
+        <v>100.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>